<commit_message>
Updated to 7.1 release
</commit_message>
<xml_diff>
--- a/Live Events Logs.xlsx
+++ b/Live Events Logs.xlsx
@@ -1,33 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22829"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsofteur-my.sharepoint.com/personal/stridout_microsoft_com/Documents/Power BI Dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsofteur-my.sharepoint.com/personal/stridout_microsoft_com/Documents/LiveEventsPBIX-master/LiveEventsPBIX-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{6E9889CE-75ED-4726-BC82-533EC9765217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{31C8089D-9829-496F-A694-3C14D4E1E9BF}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{43818A84-CA8F-43D3-AA6B-709C64EA6198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6BD33857-3969-4596-B495-F6D518363BB7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="27288" windowHeight="17664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
     <sheet name="Attendees" sheetId="2" r:id="rId2"/>
     <sheet name="QandA" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Event Title</t>
   </si>
@@ -74,7 +82,16 @@
     <t>Content</t>
   </si>
   <si>
-    <t>First Event</t>
+    <t>Introduction to Microsoft Teams</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>End Time</t>
   </si>
 </sst>
 </file>
@@ -558,10 +575,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -607,7 +626,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -621,11 +644,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{823988EE-D456-4C6E-9329-BCB807FBAACB}" name="Table1" displayName="Table1" ref="A1:B2" totalsRowShown="0">
-  <autoFilter ref="A1:B2" xr:uid="{6CB468E7-7CED-4BE9-9E7A-B04DF54F893C}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{823988EE-D456-4C6E-9329-BCB807FBAACB}" name="Table1" displayName="Table1" ref="A1:E3" totalsRowShown="0">
+  <autoFilter ref="A1:E3" xr:uid="{6CB468E7-7CED-4BE9-9E7A-B04DF54F893C}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C506C817-43D3-4810-816D-0832A5DCC84B}" name="Event ID"/>
     <tableColumn id="2" xr3:uid="{EFFDCC48-EFB3-4C43-8D73-5AA4A5DF1539}" name="Event Title"/>
+    <tableColumn id="3" xr3:uid="{D4B087F4-AFB8-4B0B-93B9-D72F0E71AD4E}" name="Date"/>
+    <tableColumn id="4" xr3:uid="{6C1B411A-E3DA-4403-8EDA-10ECBAFDAF2A}" name="Start Time"/>
+    <tableColumn id="5" xr3:uid="{BBADB6B9-32CB-4E54-8309-25FCEC0E8A31}" name="End Time"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -655,7 +681,7 @@
     <tableColumn id="1" xr3:uid="{9FDD5A12-4F24-44E9-8C3A-1485215BA30F}" name="Source"/>
     <tableColumn id="2" xr3:uid="{867AEB89-EDD2-4CE4-A9D2-5135C0FC73FD}" name="Type"/>
     <tableColumn id="3" xr3:uid="{D8644C04-B9F8-4359-AD59-41446EE27F57}" name="Identity"/>
-    <tableColumn id="4" xr3:uid="{8536B5E7-A7B6-4EA5-B2D4-8B9F91D4C8B2}" name="Timestamp"/>
+    <tableColumn id="4" xr3:uid="{8536B5E7-A7B6-4EA5-B2D4-8B9F91D4C8B2}" name="Timestamp" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{DB38497E-7666-48FD-B21E-E488AE647860}" name="Conversation Id"/>
     <tableColumn id="6" xr3:uid="{616BEAEE-60FA-4278-94C4-6B8E4DAEE42C}" name="Content"/>
     <tableColumn id="7" xr3:uid="{2E29BE69-4892-488F-953A-93BB681BCE2D}" name="Event ID"/>
@@ -927,32 +953,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.59765625" customWidth="1"/>
-    <col min="2" max="2" width="15.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
+      </c>
+      <c r="C2" s="3">
+        <v>43860</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.66666666666666663</v>
       </c>
     </row>
   </sheetData>
@@ -969,20 +1014,20 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.06640625" customWidth="1"/>
-    <col min="2" max="2" width="47.73046875" customWidth="1"/>
-    <col min="3" max="3" width="11.59765625" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="21.19921875" customWidth="1"/>
-    <col min="8" max="8" width="9.59765625" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1008,7 +1053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1032,21 +1077,21 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.06640625" style="1"/>
-    <col min="3" max="3" width="9.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.46484375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.73046875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="109.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.59765625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="2" width="9" style="1"/>
+    <col min="3" max="3" width="9.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="109.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1069,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D2" s="2"/>
     </row>
   </sheetData>

</xml_diff>